<commit_message>
Finished tkinter without threading
one by one pick up is working but not working optimally.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amal\Documents\Python36\WarehouseManagementVisualisation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Sl No.</t>
   </si>
@@ -60,25 +56,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -86,44 +83,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+  <cellXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -411,125 +381,122 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:5">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" t="n">
         <v>5.33</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:5">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" t="n">
         <v>5.33</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:5">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" t="n">
         <v>7.33</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:5">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1">
-        <v>15</v>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="n">
+        <v>8.67</v>
+      </c>
+      <c r="E5" t="n">
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:5">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1">
-        <v>15</v>
+      <c r="D6" t="n">
+        <v>8</v>
+      </c>
+      <c r="E6" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>